<commit_message>
Updates TC reporting to include target art
</commit_message>
<xml_diff>
--- a/VBA Practice/Master Roster.xlsx
+++ b/VBA Practice/Master Roster.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/svernard/Python_Practice/VBA Practice/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66FD2A86-DDA6-D345-9607-D652B9470475}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6B23D48-FBF0-7B44-A3B8-9319735CD492}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" activeTab="3" xr2:uid="{18E1EC60-5CBD-7344-9A4E-0520F0284943}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="6" xr2:uid="{18E1EC60-5CBD-7344-9A4E-0520F0284943}"/>
   </bookViews>
   <sheets>
     <sheet name="Reps Info" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13677" uniqueCount="1814">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13670" uniqueCount="1814">
   <si>
     <t>Name</t>
   </si>
@@ -14930,7 +14930,7 @@
   <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:O54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H41" sqref="H41:H55"/>
     </sheetView>
   </sheetViews>
@@ -58510,15 +58510,15 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0898F59B-444E-D148-9E60-B06AB84DEE91}">
   <sheetPr codeName="Sheet7"/>
-  <dimension ref="A1:B48"/>
+  <dimension ref="A1:B41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="28" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="57.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -58642,40 +58642,40 @@
       </c>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16" s="23" t="s">
-        <v>1770</v>
+      <c r="A16" s="24" t="s">
+        <v>1772</v>
       </c>
       <c r="B16">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:2">
-      <c r="A17" s="23" t="s">
-        <v>1770</v>
+      <c r="A17" s="20" t="s">
+        <v>1773</v>
       </c>
       <c r="B17">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="25" t="s">
+        <v>1774</v>
+      </c>
+      <c r="B18">
+        <v>18.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="20" t="s">
+        <v>1775</v>
+      </c>
+      <c r="B19">
         <v>11.5</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="23" t="s">
-        <v>1770</v>
-      </c>
-      <c r="B18">
-        <v>11.5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="24" t="s">
-        <v>1772</v>
-      </c>
-      <c r="B19">
-        <v>10</v>
-      </c>
-    </row>
     <row r="20" spans="1:2">
-      <c r="A20" s="23" t="s">
-        <v>1772</v>
+      <c r="A20" s="20" t="s">
+        <v>1776</v>
       </c>
       <c r="B20">
         <v>10</v>
@@ -58683,47 +58683,47 @@
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="20" t="s">
-        <v>1773</v>
+        <v>1777</v>
       </c>
       <c r="B21">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="20" t="s">
+        <v>1778</v>
+      </c>
+      <c r="B22">
+        <v>11.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="20" t="s">
+        <v>1779</v>
+      </c>
+      <c r="B23">
         <v>10</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" s="25" t="s">
-        <v>1774</v>
-      </c>
-      <c r="B22">
-        <v>18.5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" s="25" t="s">
-        <v>1774</v>
-      </c>
-      <c r="B23">
-        <v>18.5</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="20" t="s">
-        <v>1775</v>
+        <v>1780</v>
       </c>
       <c r="B24">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="20" t="s">
+        <v>1781</v>
+      </c>
+      <c r="B25">
         <v>11.5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25" s="25" t="s">
-        <v>1774</v>
-      </c>
-      <c r="B25">
-        <v>18.5</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="20" t="s">
-        <v>1776</v>
+        <v>1782</v>
       </c>
       <c r="B26">
         <v>10</v>
@@ -58731,182 +58731,126 @@
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="20" t="s">
-        <v>1777</v>
+        <v>1783</v>
       </c>
       <c r="B27">
-        <v>8.5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="20" t="s">
-        <v>1778</v>
+        <v>1784</v>
       </c>
       <c r="B28">
-        <v>11.5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="20" t="s">
-        <v>1779</v>
+        <v>1785</v>
       </c>
       <c r="B29">
         <v>10</v>
       </c>
     </row>
     <row r="30" spans="1:2">
-      <c r="A30" s="20" t="s">
-        <v>1780</v>
+      <c r="A30" s="25" t="s">
+        <v>1786</v>
       </c>
       <c r="B30">
         <v>10</v>
       </c>
     </row>
     <row r="31" spans="1:2">
-      <c r="A31" s="20" t="s">
-        <v>1781</v>
+      <c r="A31" s="22" t="s">
+        <v>1787</v>
       </c>
       <c r="B31">
-        <v>11.5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" s="20" t="s">
-        <v>1782</v>
+        <v>1788</v>
       </c>
       <c r="B32">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="20" t="s">
-        <v>1783</v>
+        <v>1789</v>
       </c>
       <c r="B33">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" s="20" t="s">
-        <v>1784</v>
+        <v>1790</v>
       </c>
       <c r="B34">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" s="20" t="s">
-        <v>1785</v>
+        <v>1791</v>
       </c>
       <c r="B35">
-        <v>10</v>
+        <v>10.5</v>
       </c>
     </row>
     <row r="36" spans="1:2">
-      <c r="A36" s="25" t="s">
-        <v>1786</v>
+      <c r="A36" s="20" t="s">
+        <v>1792</v>
       </c>
       <c r="B36">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="37" spans="1:2">
-      <c r="A37" s="22" t="s">
-        <v>1787</v>
+      <c r="A37" s="20" t="s">
+        <v>1793</v>
       </c>
       <c r="B37">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="38" spans="1:2">
-      <c r="A38" s="25" t="s">
-        <v>1786</v>
+      <c r="A38" s="20" t="s">
+        <v>1794</v>
       </c>
       <c r="B38">
-        <v>10</v>
+        <v>10.5</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" s="20" t="s">
-        <v>1788</v>
+        <v>1795</v>
       </c>
       <c r="B39">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" s="20" t="s">
-        <v>1789</v>
+        <v>1796</v>
       </c>
       <c r="B40">
-        <v>4</v>
+        <v>8.5</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" s="20" t="s">
-        <v>1790</v>
+        <v>1797</v>
       </c>
       <c r="B41">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2">
-      <c r="A42" s="20" t="s">
-        <v>1791</v>
-      </c>
-      <c r="B42">
-        <v>10.5</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2">
-      <c r="A43" s="20" t="s">
-        <v>1792</v>
-      </c>
-      <c r="B43">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2">
-      <c r="A44" s="20" t="s">
-        <v>1793</v>
-      </c>
-      <c r="B44">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2">
-      <c r="A45" s="20" t="s">
-        <v>1794</v>
-      </c>
-      <c r="B45">
-        <v>10.5</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2">
-      <c r="A46" s="20" t="s">
-        <v>1795</v>
-      </c>
-      <c r="B46">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2">
-      <c r="A47" s="20" t="s">
-        <v>1796</v>
-      </c>
-      <c r="B47">
-        <v>8.5</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2">
-      <c r="A48" s="20" t="s">
-        <v>1797</v>
-      </c>
-      <c r="B48">
         <v>9</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A30">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A29">
     <sortCondition ref="A2"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>